<commit_message>
Form QA1 bug fixes
</commit_message>
<xml_diff>
--- a/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FormQA1.xlsx
+++ b/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FormQA1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="QA1a (Niah)" sheetId="1" r:id="rId1"/>
@@ -1168,7 +1168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="219">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1342,9 +1342,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1427,9 +1424,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1450,13 +1444,9 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1465,6 +1455,9 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1627,6 +1620,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1672,62 +1668,62 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2382,8 +2378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B9:AH50"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="50" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:J10"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A22" zoomScaleNormal="50" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29:L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4323,41 +4319,41 @@
         <v>0</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="161"/>
-      <c r="E10" s="161"/>
-      <c r="F10" s="161"/>
-      <c r="G10" s="161"/>
-      <c r="H10" s="161"/>
-      <c r="I10" s="161"/>
-      <c r="J10" s="162"/>
-      <c r="K10" s="163"/>
-      <c r="L10" s="164"/>
-      <c r="M10" s="169" t="str">
+      <c r="D10" s="158"/>
+      <c r="E10" s="158"/>
+      <c r="F10" s="158"/>
+      <c r="G10" s="158"/>
+      <c r="H10" s="158"/>
+      <c r="I10" s="158"/>
+      <c r="J10" s="159"/>
+      <c r="K10" s="160"/>
+      <c r="L10" s="161"/>
+      <c r="M10" s="166" t="str">
         <f>'[1]Form B OLD'!J1</f>
         <v>(Project Name and Package Number)</v>
       </c>
-      <c r="N10" s="169"/>
-      <c r="O10" s="169"/>
-      <c r="P10" s="169"/>
-      <c r="Q10" s="169"/>
-      <c r="R10" s="169"/>
-      <c r="S10" s="169"/>
-      <c r="T10" s="169"/>
-      <c r="U10" s="169"/>
-      <c r="V10" s="169"/>
-      <c r="W10" s="169"/>
-      <c r="X10" s="170"/>
+      <c r="N10" s="166"/>
+      <c r="O10" s="166"/>
+      <c r="P10" s="166"/>
+      <c r="Q10" s="166"/>
+      <c r="R10" s="166"/>
+      <c r="S10" s="166"/>
+      <c r="T10" s="166"/>
+      <c r="U10" s="166"/>
+      <c r="V10" s="166"/>
+      <c r="W10" s="166"/>
+      <c r="X10" s="167"/>
       <c r="Y10" s="5"/>
-      <c r="Z10" s="173" t="s">
+      <c r="Z10" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="AA10" s="173"/>
-      <c r="AB10" s="174"/>
-      <c r="AC10" s="175" t="s">
+      <c r="AA10" s="170"/>
+      <c r="AB10" s="171"/>
+      <c r="AC10" s="172" t="s">
         <v>2</v>
       </c>
-      <c r="AD10" s="173"/>
-      <c r="AE10" s="174"/>
+      <c r="AD10" s="170"/>
+      <c r="AE10" s="171"/>
       <c r="AF10" s="6" t="s">
         <v>3</v>
       </c>
@@ -4368,147 +4364,147 @@
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="176"/>
-      <c r="F11" s="176"/>
-      <c r="G11" s="176"/>
-      <c r="H11" s="176"/>
-      <c r="I11" s="176"/>
-      <c r="J11" s="177"/>
-      <c r="K11" s="165"/>
-      <c r="L11" s="166"/>
-      <c r="M11" s="171"/>
-      <c r="N11" s="171"/>
-      <c r="O11" s="171"/>
-      <c r="P11" s="171"/>
-      <c r="Q11" s="171"/>
-      <c r="R11" s="171"/>
-      <c r="S11" s="171"/>
-      <c r="T11" s="171"/>
-      <c r="U11" s="171"/>
-      <c r="V11" s="171"/>
-      <c r="W11" s="171"/>
-      <c r="X11" s="172"/>
+      <c r="E11" s="173"/>
+      <c r="F11" s="173"/>
+      <c r="G11" s="173"/>
+      <c r="H11" s="173"/>
+      <c r="I11" s="173"/>
+      <c r="J11" s="174"/>
+      <c r="K11" s="162"/>
+      <c r="L11" s="163"/>
+      <c r="M11" s="168"/>
+      <c r="N11" s="168"/>
+      <c r="O11" s="168"/>
+      <c r="P11" s="168"/>
+      <c r="Q11" s="168"/>
+      <c r="R11" s="168"/>
+      <c r="S11" s="168"/>
+      <c r="T11" s="168"/>
+      <c r="U11" s="168"/>
+      <c r="V11" s="168"/>
+      <c r="W11" s="168"/>
+      <c r="X11" s="169"/>
       <c r="Y11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="Z11" s="140"/>
-      <c r="AA11" s="140"/>
-      <c r="AB11" s="178"/>
-      <c r="AC11" s="179"/>
-      <c r="AD11" s="140"/>
-      <c r="AE11" s="178"/>
-      <c r="AF11" s="143"/>
+      <c r="Z11" s="137"/>
+      <c r="AA11" s="137"/>
+      <c r="AB11" s="175"/>
+      <c r="AC11" s="176"/>
+      <c r="AD11" s="137"/>
+      <c r="AE11" s="175"/>
+      <c r="AF11" s="140"/>
       <c r="AG11" s="12"/>
       <c r="AH11" s="12"/>
     </row>
     <row r="12" spans="2:34" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="144" t="s">
+      <c r="B12" s="141" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="145"/>
-      <c r="D12" s="145"/>
-      <c r="E12" s="146"/>
-      <c r="F12" s="146"/>
-      <c r="G12" s="146"/>
-      <c r="H12" s="146"/>
-      <c r="I12" s="146"/>
-      <c r="J12" s="147"/>
-      <c r="K12" s="165"/>
-      <c r="L12" s="166"/>
-      <c r="M12" s="148" t="s">
+      <c r="C12" s="142"/>
+      <c r="D12" s="142"/>
+      <c r="E12" s="143"/>
+      <c r="F12" s="143"/>
+      <c r="G12" s="143"/>
+      <c r="H12" s="143"/>
+      <c r="I12" s="143"/>
+      <c r="J12" s="144"/>
+      <c r="K12" s="162"/>
+      <c r="L12" s="163"/>
+      <c r="M12" s="145" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="148"/>
-      <c r="O12" s="148"/>
-      <c r="P12" s="148"/>
-      <c r="Q12" s="148"/>
-      <c r="R12" s="148"/>
-      <c r="S12" s="148"/>
-      <c r="T12" s="148"/>
-      <c r="U12" s="148"/>
-      <c r="V12" s="148"/>
-      <c r="W12" s="148"/>
-      <c r="X12" s="149"/>
+      <c r="N12" s="145"/>
+      <c r="O12" s="145"/>
+      <c r="P12" s="145"/>
+      <c r="Q12" s="145"/>
+      <c r="R12" s="145"/>
+      <c r="S12" s="145"/>
+      <c r="T12" s="145"/>
+      <c r="U12" s="145"/>
+      <c r="V12" s="145"/>
+      <c r="W12" s="145"/>
+      <c r="X12" s="146"/>
       <c r="Y12" s="13"/>
-      <c r="Z12" s="140"/>
-      <c r="AA12" s="140"/>
-      <c r="AB12" s="178"/>
-      <c r="AC12" s="179"/>
-      <c r="AD12" s="140"/>
-      <c r="AE12" s="178"/>
-      <c r="AF12" s="143"/>
+      <c r="Z12" s="137"/>
+      <c r="AA12" s="137"/>
+      <c r="AB12" s="175"/>
+      <c r="AC12" s="176"/>
+      <c r="AD12" s="137"/>
+      <c r="AE12" s="175"/>
+      <c r="AF12" s="140"/>
       <c r="AG12" s="12"/>
       <c r="AH12" s="12"/>
     </row>
     <row r="13" spans="2:34" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="152"/>
-      <c r="C13" s="133"/>
-      <c r="D13" s="133"/>
-      <c r="E13" s="133"/>
-      <c r="F13" s="133"/>
-      <c r="G13" s="133"/>
-      <c r="H13" s="133"/>
-      <c r="I13" s="133"/>
-      <c r="J13" s="153"/>
-      <c r="K13" s="165"/>
-      <c r="L13" s="166"/>
-      <c r="M13" s="148"/>
-      <c r="N13" s="148"/>
-      <c r="O13" s="148"/>
-      <c r="P13" s="148"/>
-      <c r="Q13" s="148"/>
-      <c r="R13" s="148"/>
-      <c r="S13" s="148"/>
-      <c r="T13" s="148"/>
-      <c r="U13" s="148"/>
-      <c r="V13" s="148"/>
-      <c r="W13" s="148"/>
-      <c r="X13" s="149"/>
+      <c r="B13" s="149"/>
+      <c r="C13" s="130"/>
+      <c r="D13" s="130"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="130"/>
+      <c r="G13" s="130"/>
+      <c r="H13" s="130"/>
+      <c r="I13" s="130"/>
+      <c r="J13" s="150"/>
+      <c r="K13" s="162"/>
+      <c r="L13" s="163"/>
+      <c r="M13" s="145"/>
+      <c r="N13" s="145"/>
+      <c r="O13" s="145"/>
+      <c r="P13" s="145"/>
+      <c r="Q13" s="145"/>
+      <c r="R13" s="145"/>
+      <c r="S13" s="145"/>
+      <c r="T13" s="145"/>
+      <c r="U13" s="145"/>
+      <c r="V13" s="145"/>
+      <c r="W13" s="145"/>
+      <c r="X13" s="146"/>
       <c r="Y13" s="14"/>
-      <c r="Z13" s="140"/>
-      <c r="AA13" s="140"/>
-      <c r="AB13" s="178"/>
-      <c r="AC13" s="179"/>
-      <c r="AD13" s="140"/>
-      <c r="AE13" s="178"/>
-      <c r="AF13" s="143"/>
+      <c r="Z13" s="137"/>
+      <c r="AA13" s="137"/>
+      <c r="AB13" s="175"/>
+      <c r="AC13" s="176"/>
+      <c r="AD13" s="137"/>
+      <c r="AE13" s="175"/>
+      <c r="AF13" s="140"/>
       <c r="AG13" s="12"/>
       <c r="AH13" s="12"/>
     </row>
     <row r="14" spans="2:34" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="154"/>
-      <c r="C14" s="155"/>
-      <c r="D14" s="155"/>
-      <c r="E14" s="155"/>
-      <c r="F14" s="155"/>
-      <c r="G14" s="155"/>
-      <c r="H14" s="155"/>
-      <c r="I14" s="155"/>
-      <c r="J14" s="156"/>
-      <c r="K14" s="167"/>
-      <c r="L14" s="168"/>
-      <c r="M14" s="150"/>
-      <c r="N14" s="150"/>
-      <c r="O14" s="150"/>
-      <c r="P14" s="150"/>
-      <c r="Q14" s="150"/>
-      <c r="R14" s="150"/>
-      <c r="S14" s="150"/>
-      <c r="T14" s="150"/>
-      <c r="U14" s="150"/>
-      <c r="V14" s="150"/>
-      <c r="W14" s="150"/>
-      <c r="X14" s="151"/>
+      <c r="B14" s="151"/>
+      <c r="C14" s="152"/>
+      <c r="D14" s="152"/>
+      <c r="E14" s="152"/>
+      <c r="F14" s="152"/>
+      <c r="G14" s="152"/>
+      <c r="H14" s="152"/>
+      <c r="I14" s="152"/>
+      <c r="J14" s="153"/>
+      <c r="K14" s="164"/>
+      <c r="L14" s="165"/>
+      <c r="M14" s="147"/>
+      <c r="N14" s="147"/>
+      <c r="O14" s="147"/>
+      <c r="P14" s="147"/>
+      <c r="Q14" s="147"/>
+      <c r="R14" s="147"/>
+      <c r="S14" s="147"/>
+      <c r="T14" s="147"/>
+      <c r="U14" s="147"/>
+      <c r="V14" s="147"/>
+      <c r="W14" s="147"/>
+      <c r="X14" s="148"/>
       <c r="Y14" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="Z14" s="140"/>
-      <c r="AA14" s="140"/>
-      <c r="AB14" s="178"/>
-      <c r="AC14" s="179"/>
-      <c r="AD14" s="140"/>
-      <c r="AE14" s="178"/>
-      <c r="AF14" s="143"/>
+      <c r="Z14" s="137"/>
+      <c r="AA14" s="137"/>
+      <c r="AB14" s="175"/>
+      <c r="AC14" s="176"/>
+      <c r="AD14" s="137"/>
+      <c r="AE14" s="175"/>
+      <c r="AF14" s="140"/>
       <c r="AG14" s="12"/>
       <c r="AH14" s="12"/>
     </row>
@@ -4518,41 +4514,41 @@
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
-      <c r="E15" s="141"/>
-      <c r="F15" s="141"/>
-      <c r="G15" s="138" t="s">
+      <c r="E15" s="138"/>
+      <c r="F15" s="138"/>
+      <c r="G15" s="135" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="139"/>
-      <c r="I15" s="139"/>
-      <c r="J15" s="139"/>
-      <c r="K15" s="139"/>
-      <c r="L15" s="142"/>
+      <c r="H15" s="136"/>
+      <c r="I15" s="136"/>
+      <c r="J15" s="136"/>
+      <c r="K15" s="136"/>
+      <c r="L15" s="139"/>
       <c r="M15" s="18"/>
       <c r="N15" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="O15" s="141"/>
-      <c r="P15" s="141"/>
-      <c r="Q15" s="138" t="s">
+      <c r="O15" s="138"/>
+      <c r="P15" s="138"/>
+      <c r="Q15" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="R15" s="139"/>
-      <c r="S15" s="139"/>
-      <c r="T15" s="139"/>
-      <c r="U15" s="139"/>
-      <c r="V15" s="139"/>
-      <c r="W15" s="139"/>
-      <c r="X15" s="157"/>
+      <c r="R15" s="136"/>
+      <c r="S15" s="136"/>
+      <c r="T15" s="136"/>
+      <c r="U15" s="136"/>
+      <c r="V15" s="136"/>
+      <c r="W15" s="136"/>
+      <c r="X15" s="154"/>
       <c r="Y15" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="Z15" s="158"/>
-      <c r="AA15" s="158"/>
-      <c r="AB15" s="159"/>
-      <c r="AC15" s="160"/>
-      <c r="AD15" s="158"/>
-      <c r="AE15" s="159"/>
+      <c r="Z15" s="155"/>
+      <c r="AA15" s="155"/>
+      <c r="AB15" s="156"/>
+      <c r="AC15" s="157"/>
+      <c r="AD15" s="155"/>
+      <c r="AE15" s="156"/>
       <c r="AF15" s="21"/>
     </row>
     <row r="16" spans="2:34" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -4612,10 +4608,10 @@
       <c r="J17" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="134" t="s">
+      <c r="K17" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="L17" s="135"/>
+      <c r="L17" s="132"/>
       <c r="M17" s="27"/>
       <c r="N17" s="28"/>
       <c r="O17" s="28"/>
@@ -4649,8 +4645,8 @@
       <c r="J18" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="134"/>
-      <c r="L18" s="135"/>
+      <c r="K18" s="131"/>
+      <c r="L18" s="132"/>
       <c r="M18" s="35">
         <v>1</v>
       </c>
@@ -4705,8 +4701,8 @@
       <c r="H19" s="45"/>
       <c r="I19" s="28"/>
       <c r="J19" s="31"/>
-      <c r="K19" s="136"/>
-      <c r="L19" s="137"/>
+      <c r="K19" s="133"/>
+      <c r="L19" s="134"/>
       <c r="M19" s="35"/>
       <c r="N19" s="36"/>
       <c r="O19" s="36"/>
@@ -4724,7 +4720,7 @@
       <c r="AA19" s="41"/>
       <c r="AB19" s="39"/>
       <c r="AC19" s="28"/>
-      <c r="AD19" s="100"/>
+      <c r="AD19" s="99"/>
       <c r="AF19" s="48"/>
     </row>
     <row r="20" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4741,8 +4737,8 @@
       <c r="H20" s="28"/>
       <c r="I20" s="28"/>
       <c r="J20" s="31"/>
-      <c r="K20" s="136"/>
-      <c r="L20" s="137"/>
+      <c r="K20" s="133"/>
+      <c r="L20" s="134"/>
       <c r="M20" s="49">
         <v>2</v>
       </c>
@@ -4778,7 +4774,7 @@
         <v>40</v>
       </c>
       <c r="AC20" s="28"/>
-      <c r="AD20" s="99"/>
+      <c r="AD20" s="98"/>
       <c r="AF20" s="52"/>
     </row>
     <row r="21" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4795,8 +4791,8 @@
       <c r="H21" s="54"/>
       <c r="I21" s="28"/>
       <c r="J21" s="31"/>
-      <c r="K21" s="136"/>
-      <c r="L21" s="137"/>
+      <c r="K21" s="133"/>
+      <c r="L21" s="134"/>
       <c r="M21" s="49"/>
       <c r="N21" s="36"/>
       <c r="O21" s="36"/>
@@ -4831,8 +4827,8 @@
       <c r="H22" s="54"/>
       <c r="I22" s="28"/>
       <c r="J22" s="31"/>
-      <c r="K22" s="136"/>
-      <c r="L22" s="137"/>
+      <c r="K22" s="133"/>
+      <c r="L22" s="134"/>
       <c r="M22" s="35">
         <v>3</v>
       </c>
@@ -4870,7 +4866,7 @@
         <v>33</v>
       </c>
       <c r="AC22" s="28"/>
-      <c r="AD22" s="99"/>
+      <c r="AD22" s="98"/>
       <c r="AE22" s="28"/>
       <c r="AF22" s="55"/>
     </row>
@@ -4888,8 +4884,8 @@
       <c r="H23" s="54"/>
       <c r="I23" s="28"/>
       <c r="J23" s="31"/>
-      <c r="K23" s="136"/>
-      <c r="L23" s="137"/>
+      <c r="K23" s="133"/>
+      <c r="L23" s="134"/>
       <c r="M23" s="35"/>
       <c r="N23" s="36"/>
       <c r="O23" s="36"/>
@@ -4958,7 +4954,7 @@
         <v>40</v>
       </c>
       <c r="AC24" s="28"/>
-      <c r="AD24" s="99"/>
+      <c r="AD24" s="98"/>
       <c r="AF24" s="52"/>
     </row>
     <row r="25" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5037,7 +5033,7 @@
         <v>33</v>
       </c>
       <c r="AC26" s="28"/>
-      <c r="AD26" s="99"/>
+      <c r="AD26" s="98"/>
       <c r="AE26" s="28"/>
       <c r="AF26" s="52"/>
     </row>
@@ -5064,10 +5060,10 @@
     </row>
     <row r="28" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="70"/>
-      <c r="C28" s="140" t="s">
+      <c r="C28" s="137" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="140"/>
+      <c r="D28" s="137"/>
       <c r="E28" s="51"/>
       <c r="F28" s="71" t="s">
         <v>50</v>
@@ -5075,10 +5071,10 @@
       <c r="H28" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="J28" s="140" t="s">
+      <c r="J28" s="137" t="s">
         <v>52</v>
       </c>
-      <c r="K28" s="140"/>
+      <c r="K28" s="137"/>
       <c r="L28" s="72" t="s">
         <v>21</v>
       </c>
@@ -5117,7 +5113,7 @@
         <v>33</v>
       </c>
       <c r="AC28" s="28"/>
-      <c r="AD28" s="99"/>
+      <c r="AD28" s="98"/>
       <c r="AE28" s="28"/>
       <c r="AF28" s="55"/>
     </row>
@@ -5125,16 +5121,16 @@
       <c r="B29" s="27">
         <v>1</v>
       </c>
-      <c r="C29" s="131"/>
-      <c r="D29" s="131"/>
+      <c r="C29" s="128"/>
+      <c r="D29" s="128"/>
       <c r="E29" s="28"/>
       <c r="F29" s="45"/>
       <c r="G29" s="28"/>
       <c r="H29" s="28"/>
       <c r="I29" s="28"/>
-      <c r="J29" s="133"/>
-      <c r="K29" s="133"/>
-      <c r="L29" s="73"/>
+      <c r="J29" s="130"/>
+      <c r="K29" s="130"/>
+      <c r="L29" s="122"/>
       <c r="M29" s="35"/>
       <c r="N29" s="36"/>
       <c r="O29" s="36"/>
@@ -5160,16 +5156,16 @@
       <c r="B30" s="27">
         <v>2</v>
       </c>
-      <c r="C30" s="132"/>
-      <c r="D30" s="132"/>
+      <c r="C30" s="129"/>
+      <c r="D30" s="129"/>
       <c r="E30" s="28"/>
       <c r="F30" s="45"/>
       <c r="G30" s="28"/>
       <c r="H30" s="53"/>
       <c r="I30" s="28"/>
-      <c r="J30" s="133"/>
-      <c r="K30" s="133"/>
-      <c r="L30" s="73"/>
+      <c r="J30" s="130"/>
+      <c r="K30" s="130"/>
+      <c r="L30" s="122"/>
       <c r="M30" s="35">
         <v>7</v>
       </c>
@@ -5178,7 +5174,7 @@
       </c>
       <c r="O30" s="36"/>
       <c r="P30" s="37"/>
-      <c r="Q30" s="74" t="s">
+      <c r="Q30" s="73" t="s">
         <v>26</v>
       </c>
       <c r="R30" s="39" t="s">
@@ -5205,7 +5201,7 @@
         <v>33</v>
       </c>
       <c r="AC30" s="28"/>
-      <c r="AD30" s="99"/>
+      <c r="AD30" s="98"/>
       <c r="AE30" s="28"/>
       <c r="AF30" s="55"/>
     </row>
@@ -5213,16 +5209,16 @@
       <c r="B31" s="27">
         <v>3</v>
       </c>
-      <c r="C31" s="132"/>
-      <c r="D31" s="132"/>
+      <c r="C31" s="129"/>
+      <c r="D31" s="129"/>
       <c r="E31" s="28"/>
       <c r="F31" s="28"/>
       <c r="G31" s="28"/>
       <c r="H31" s="53"/>
       <c r="I31" s="28"/>
-      <c r="J31" s="133"/>
-      <c r="K31" s="133"/>
-      <c r="L31" s="73"/>
+      <c r="J31" s="130"/>
+      <c r="K31" s="130"/>
+      <c r="L31" s="122"/>
       <c r="M31" s="62"/>
       <c r="N31" s="62"/>
       <c r="O31" s="62"/>
@@ -5238,16 +5234,16 @@
       <c r="B32" s="27">
         <v>4</v>
       </c>
-      <c r="C32" s="132"/>
-      <c r="D32" s="132"/>
+      <c r="C32" s="129"/>
+      <c r="D32" s="129"/>
       <c r="E32" s="28"/>
       <c r="F32" s="54"/>
       <c r="G32" s="28"/>
       <c r="H32" s="54"/>
       <c r="I32" s="28"/>
-      <c r="J32" s="133"/>
-      <c r="K32" s="133"/>
-      <c r="L32" s="73"/>
+      <c r="J32" s="130"/>
+      <c r="K32" s="130"/>
+      <c r="L32" s="122"/>
       <c r="M32" s="49">
         <v>8</v>
       </c>
@@ -5256,7 +5252,7 @@
       </c>
       <c r="O32" s="36"/>
       <c r="P32" s="39"/>
-      <c r="Q32" s="74" t="s">
+      <c r="Q32" s="73" t="s">
         <v>26</v>
       </c>
       <c r="R32" s="39" t="s">
@@ -5284,54 +5280,54 @@
       <c r="B33" s="27">
         <v>5</v>
       </c>
-      <c r="C33" s="132"/>
-      <c r="D33" s="132"/>
+      <c r="C33" s="129"/>
+      <c r="D33" s="129"/>
       <c r="E33" s="28"/>
       <c r="F33" s="54"/>
       <c r="G33" s="28"/>
       <c r="H33" s="54"/>
       <c r="I33" s="28"/>
-      <c r="J33" s="133"/>
-      <c r="K33" s="133"/>
-      <c r="L33" s="73"/>
+      <c r="J33" s="130"/>
+      <c r="K33" s="130"/>
+      <c r="L33" s="122"/>
       <c r="AF33" s="44"/>
     </row>
     <row r="34" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="27">
         <v>6</v>
       </c>
-      <c r="C34" s="129"/>
-      <c r="D34" s="129"/>
+      <c r="C34" s="126"/>
+      <c r="D34" s="126"/>
       <c r="E34" s="28"/>
       <c r="F34" s="54"/>
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
       <c r="I34" s="28"/>
-      <c r="J34" s="133"/>
-      <c r="K34" s="133"/>
-      <c r="L34" s="73"/>
+      <c r="J34" s="130"/>
+      <c r="K34" s="130"/>
+      <c r="L34" s="122"/>
       <c r="AF34" s="44"/>
     </row>
     <row r="35" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="27">
         <v>7</v>
       </c>
-      <c r="C35" s="131"/>
-      <c r="D35" s="131"/>
+      <c r="C35" s="128"/>
+      <c r="D35" s="128"/>
       <c r="E35" s="28"/>
       <c r="F35" s="54"/>
       <c r="G35" s="28"/>
       <c r="H35" s="54"/>
       <c r="I35" s="28"/>
-      <c r="J35" s="133"/>
-      <c r="K35" s="133"/>
-      <c r="L35" s="73"/>
-      <c r="M35" s="75"/>
-      <c r="N35" s="76"/>
-      <c r="O35" s="77"/>
-      <c r="P35" s="78"/>
-      <c r="Q35" s="79"/>
-      <c r="R35" s="80"/>
+      <c r="J35" s="130"/>
+      <c r="K35" s="130"/>
+      <c r="L35" s="122"/>
+      <c r="M35" s="74"/>
+      <c r="N35" s="75"/>
+      <c r="O35" s="76"/>
+      <c r="P35" s="77"/>
+      <c r="Q35" s="78"/>
+      <c r="R35" s="79"/>
       <c r="S35" s="28"/>
       <c r="T35" s="28"/>
       <c r="U35" s="31"/>
@@ -5350,16 +5346,16 @@
       <c r="B36" s="27">
         <v>8</v>
       </c>
-      <c r="C36" s="129"/>
-      <c r="D36" s="129"/>
+      <c r="C36" s="126"/>
+      <c r="D36" s="126"/>
       <c r="E36" s="28"/>
       <c r="F36" s="28"/>
       <c r="G36" s="28"/>
       <c r="H36" s="54"/>
       <c r="I36" s="28"/>
-      <c r="J36" s="133"/>
-      <c r="K36" s="133"/>
-      <c r="L36" s="73"/>
+      <c r="J36" s="130"/>
+      <c r="K36" s="130"/>
+      <c r="L36" s="122"/>
       <c r="M36" s="31"/>
       <c r="N36" s="70"/>
       <c r="R36" s="44"/>
@@ -5367,21 +5363,21 @@
     </row>
     <row r="37" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="27"/>
-      <c r="C37" s="81"/>
-      <c r="D37" s="81"/>
+      <c r="C37" s="80"/>
+      <c r="D37" s="80"/>
       <c r="E37" s="28"/>
       <c r="F37" s="53"/>
       <c r="G37" s="28"/>
       <c r="H37" s="28"/>
       <c r="I37" s="28"/>
-      <c r="J37" s="82"/>
+      <c r="J37" s="81"/>
       <c r="K37" s="39"/>
-      <c r="L37" s="83"/>
-      <c r="N37" s="84"/>
-      <c r="O37" s="85"/>
-      <c r="P37" s="85"/>
-      <c r="Q37" s="85"/>
-      <c r="R37" s="86"/>
+      <c r="L37" s="82"/>
+      <c r="N37" s="83"/>
+      <c r="O37" s="84"/>
+      <c r="P37" s="84"/>
+      <c r="Q37" s="84"/>
+      <c r="R37" s="85"/>
       <c r="AF37" s="44"/>
     </row>
     <row r="38" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5394,12 +5390,12 @@
       <c r="H38" s="60"/>
       <c r="I38" s="60"/>
       <c r="J38" s="60"/>
-      <c r="K38" s="87"/>
+      <c r="K38" s="86"/>
       <c r="L38" s="61"/>
-      <c r="M38" s="84"/>
-      <c r="U38" s="85"/>
-      <c r="X38" s="85"/>
-      <c r="Y38" s="85"/>
+      <c r="M38" s="83"/>
+      <c r="U38" s="84"/>
+      <c r="X38" s="84"/>
+      <c r="Y38" s="84"/>
       <c r="AF38" s="44"/>
     </row>
     <row r="39" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5423,7 +5419,7 @@
         <v>61</v>
       </c>
       <c r="O39" s="65"/>
-      <c r="P39" s="88"/>
+      <c r="P39" s="87"/>
       <c r="Q39" s="66"/>
       <c r="R39" s="66"/>
       <c r="S39" s="66"/>
@@ -5431,7 +5427,7 @@
       <c r="U39" s="66"/>
       <c r="V39" s="66"/>
       <c r="W39" s="66"/>
-      <c r="X39" s="89"/>
+      <c r="X39" s="88"/>
       <c r="Y39" s="66"/>
       <c r="Z39" s="66"/>
       <c r="AA39" s="66"/>
@@ -5443,12 +5439,12 @@
     </row>
     <row r="40" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="27"/>
-      <c r="C40" s="134" t="s">
+      <c r="C40" s="131" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="134"/>
+      <c r="D40" s="131"/>
       <c r="E40" s="28"/>
-      <c r="F40" s="134" t="s">
+      <c r="F40" s="131" t="s">
         <v>62</v>
       </c>
       <c r="H40" s="28"/>
@@ -5457,7 +5453,7 @@
         <v>20</v>
       </c>
       <c r="K40" s="28"/>
-      <c r="L40" s="135" t="s">
+      <c r="L40" s="132" t="s">
         <v>21</v>
       </c>
       <c r="M40" s="27"/>
@@ -5471,49 +5467,49 @@
       <c r="U40" s="28"/>
       <c r="V40" s="28"/>
       <c r="W40" s="28"/>
-      <c r="X40" s="90" t="s">
+      <c r="X40" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="Y40" s="91"/>
-      <c r="Z40" s="91"/>
-      <c r="AC40" s="91"/>
+      <c r="Y40" s="90"/>
+      <c r="Z40" s="90"/>
+      <c r="AC40" s="90"/>
       <c r="AF40" s="44"/>
     </row>
     <row r="41" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="27"/>
-      <c r="C41" s="134"/>
-      <c r="D41" s="134"/>
+      <c r="C41" s="131"/>
+      <c r="D41" s="131"/>
       <c r="E41" s="28"/>
-      <c r="F41" s="134"/>
+      <c r="F41" s="131"/>
       <c r="H41" s="28"/>
       <c r="I41" s="28"/>
       <c r="J41" s="29" t="s">
         <v>63</v>
       </c>
       <c r="K41" s="28"/>
-      <c r="L41" s="135"/>
-      <c r="M41" s="75">
+      <c r="L41" s="132"/>
+      <c r="M41" s="74">
         <v>1</v>
       </c>
       <c r="N41" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="P41" s="92"/>
+      <c r="P41" s="91"/>
       <c r="Q41" s="28"/>
       <c r="R41" s="28"/>
-      <c r="S41" s="127"/>
-      <c r="T41" s="127"/>
-      <c r="U41" s="127"/>
-      <c r="V41" s="93"/>
-      <c r="W41" s="93"/>
-      <c r="X41" s="128"/>
-      <c r="Y41" s="128"/>
-      <c r="Z41" s="128"/>
-      <c r="AA41" s="128"/>
-      <c r="AB41" s="128"/>
-      <c r="AC41" s="128"/>
-      <c r="AD41" s="128"/>
-      <c r="AE41" s="128"/>
+      <c r="S41" s="124"/>
+      <c r="T41" s="124"/>
+      <c r="U41" s="124"/>
+      <c r="V41" s="92"/>
+      <c r="W41" s="92"/>
+      <c r="X41" s="125"/>
+      <c r="Y41" s="125"/>
+      <c r="Z41" s="125"/>
+      <c r="AA41" s="125"/>
+      <c r="AB41" s="125"/>
+      <c r="AC41" s="125"/>
+      <c r="AD41" s="125"/>
+      <c r="AE41" s="125"/>
       <c r="AF41" s="44"/>
     </row>
     <row r="42" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5528,7 +5524,7 @@
       <c r="J42" s="28"/>
       <c r="K42" s="28"/>
       <c r="L42" s="28"/>
-      <c r="M42" s="75"/>
+      <c r="M42" s="74"/>
       <c r="N42" s="28"/>
       <c r="O42" s="28"/>
       <c r="P42" s="32"/>
@@ -5539,22 +5535,22 @@
       <c r="U42" s="28"/>
       <c r="V42" s="28"/>
       <c r="W42" s="28"/>
-      <c r="X42" s="126"/>
-      <c r="Y42" s="126"/>
-      <c r="Z42" s="126"/>
-      <c r="AA42" s="126"/>
-      <c r="AB42" s="126"/>
-      <c r="AC42" s="126"/>
-      <c r="AD42" s="126"/>
-      <c r="AE42" s="126"/>
+      <c r="X42" s="123"/>
+      <c r="Y42" s="123"/>
+      <c r="Z42" s="123"/>
+      <c r="AA42" s="123"/>
+      <c r="AB42" s="123"/>
+      <c r="AC42" s="123"/>
+      <c r="AD42" s="123"/>
+      <c r="AE42" s="123"/>
       <c r="AF42" s="44"/>
     </row>
     <row r="43" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="27">
         <v>1</v>
       </c>
-      <c r="C43" s="130"/>
-      <c r="D43" s="130"/>
+      <c r="C43" s="127"/>
+      <c r="D43" s="127"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
@@ -5563,122 +5559,122 @@
       <c r="J43" s="31"/>
       <c r="K43" s="28"/>
       <c r="L43" s="52"/>
-      <c r="M43" s="94">
+      <c r="M43" s="93">
         <v>2</v>
       </c>
       <c r="N43" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="S43" s="127"/>
-      <c r="T43" s="127"/>
-      <c r="U43" s="127"/>
+      <c r="S43" s="124"/>
+      <c r="T43" s="124"/>
+      <c r="U43" s="124"/>
       <c r="V43" s="71"/>
-      <c r="X43" s="128"/>
-      <c r="Y43" s="128"/>
-      <c r="Z43" s="128"/>
-      <c r="AA43" s="128"/>
-      <c r="AB43" s="128"/>
-      <c r="AC43" s="128"/>
-      <c r="AD43" s="128"/>
-      <c r="AE43" s="128"/>
+      <c r="X43" s="125"/>
+      <c r="Y43" s="125"/>
+      <c r="Z43" s="125"/>
+      <c r="AA43" s="125"/>
+      <c r="AB43" s="125"/>
+      <c r="AC43" s="125"/>
+      <c r="AD43" s="125"/>
+      <c r="AE43" s="125"/>
       <c r="AF43" s="44"/>
     </row>
     <row r="44" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="70">
         <v>2</v>
       </c>
-      <c r="C44" s="131"/>
-      <c r="D44" s="131"/>
+      <c r="C44" s="128"/>
+      <c r="D44" s="128"/>
       <c r="F44" s="54"/>
       <c r="J44" s="31"/>
       <c r="L44" s="55"/>
-      <c r="M44" s="94"/>
-      <c r="X44" s="126"/>
-      <c r="Y44" s="126"/>
-      <c r="Z44" s="126"/>
-      <c r="AA44" s="126"/>
-      <c r="AB44" s="126"/>
-      <c r="AC44" s="126"/>
-      <c r="AD44" s="126"/>
-      <c r="AE44" s="126"/>
+      <c r="M44" s="93"/>
+      <c r="X44" s="123"/>
+      <c r="Y44" s="123"/>
+      <c r="Z44" s="123"/>
+      <c r="AA44" s="123"/>
+      <c r="AB44" s="123"/>
+      <c r="AC44" s="123"/>
+      <c r="AD44" s="123"/>
+      <c r="AE44" s="123"/>
       <c r="AF44" s="44"/>
     </row>
     <row r="45" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="70">
         <v>3</v>
       </c>
-      <c r="C45" s="129"/>
-      <c r="D45" s="129"/>
+      <c r="C45" s="126"/>
+      <c r="D45" s="126"/>
       <c r="F45" s="28"/>
       <c r="J45" s="31"/>
-      <c r="L45" s="95"/>
-      <c r="M45" s="94">
+      <c r="L45" s="94"/>
+      <c r="M45" s="93">
         <v>3</v>
       </c>
       <c r="N45" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="S45" s="127"/>
-      <c r="T45" s="127"/>
-      <c r="U45" s="127"/>
+      <c r="S45" s="124"/>
+      <c r="T45" s="124"/>
+      <c r="U45" s="124"/>
       <c r="V45" s="71"/>
-      <c r="X45" s="128"/>
-      <c r="Y45" s="128"/>
-      <c r="Z45" s="128"/>
-      <c r="AA45" s="128"/>
-      <c r="AB45" s="128"/>
-      <c r="AC45" s="128"/>
-      <c r="AD45" s="128"/>
-      <c r="AE45" s="128"/>
+      <c r="X45" s="125"/>
+      <c r="Y45" s="125"/>
+      <c r="Z45" s="125"/>
+      <c r="AA45" s="125"/>
+      <c r="AB45" s="125"/>
+      <c r="AC45" s="125"/>
+      <c r="AD45" s="125"/>
+      <c r="AE45" s="125"/>
       <c r="AF45" s="44"/>
     </row>
     <row r="46" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="27">
         <v>4</v>
       </c>
-      <c r="C46" s="129"/>
-      <c r="D46" s="129"/>
+      <c r="C46" s="126"/>
+      <c r="D46" s="126"/>
       <c r="F46" s="54"/>
       <c r="J46" s="31"/>
       <c r="L46" s="55"/>
-      <c r="M46" s="94"/>
-      <c r="X46" s="126"/>
-      <c r="Y46" s="126"/>
-      <c r="Z46" s="126"/>
-      <c r="AA46" s="126"/>
-      <c r="AB46" s="126"/>
-      <c r="AC46" s="126"/>
-      <c r="AD46" s="126"/>
-      <c r="AE46" s="126"/>
+      <c r="M46" s="93"/>
+      <c r="X46" s="123"/>
+      <c r="Y46" s="123"/>
+      <c r="Z46" s="123"/>
+      <c r="AA46" s="123"/>
+      <c r="AB46" s="123"/>
+      <c r="AC46" s="123"/>
+      <c r="AD46" s="123"/>
+      <c r="AE46" s="123"/>
       <c r="AF46" s="44"/>
     </row>
     <row r="47" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="27">
         <v>5</v>
       </c>
-      <c r="C47" s="129"/>
-      <c r="D47" s="129"/>
+      <c r="C47" s="126"/>
+      <c r="D47" s="126"/>
       <c r="F47" s="28"/>
       <c r="J47" s="31"/>
-      <c r="L47" s="95"/>
-      <c r="M47" s="94">
+      <c r="L47" s="94"/>
+      <c r="M47" s="93">
         <v>4</v>
       </c>
       <c r="N47" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="S47" s="127"/>
-      <c r="T47" s="127"/>
-      <c r="U47" s="127"/>
+      <c r="S47" s="124"/>
+      <c r="T47" s="124"/>
+      <c r="U47" s="124"/>
       <c r="V47" s="71"/>
-      <c r="X47" s="128"/>
-      <c r="Y47" s="128"/>
-      <c r="Z47" s="128"/>
-      <c r="AA47" s="128"/>
-      <c r="AB47" s="128"/>
-      <c r="AC47" s="128"/>
-      <c r="AD47" s="128"/>
-      <c r="AE47" s="128"/>
+      <c r="X47" s="125"/>
+      <c r="Y47" s="125"/>
+      <c r="Z47" s="125"/>
+      <c r="AA47" s="125"/>
+      <c r="AB47" s="125"/>
+      <c r="AC47" s="125"/>
+      <c r="AD47" s="125"/>
+      <c r="AE47" s="125"/>
       <c r="AF47" s="44"/>
     </row>
     <row r="48" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5686,85 +5682,85 @@
       <c r="F48" s="47"/>
       <c r="J48" s="31"/>
       <c r="L48" s="44"/>
-      <c r="M48" s="94"/>
-      <c r="X48" s="126"/>
-      <c r="Y48" s="126"/>
-      <c r="Z48" s="126"/>
-      <c r="AA48" s="126"/>
-      <c r="AB48" s="126"/>
-      <c r="AC48" s="126"/>
-      <c r="AD48" s="126"/>
-      <c r="AE48" s="126"/>
+      <c r="M48" s="93"/>
+      <c r="X48" s="123"/>
+      <c r="Y48" s="123"/>
+      <c r="Z48" s="123"/>
+      <c r="AA48" s="123"/>
+      <c r="AB48" s="123"/>
+      <c r="AC48" s="123"/>
+      <c r="AD48" s="123"/>
+      <c r="AE48" s="123"/>
       <c r="AF48" s="44"/>
     </row>
     <row r="49" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="84"/>
-      <c r="C49" s="85"/>
-      <c r="D49" s="85"/>
-      <c r="E49" s="85"/>
-      <c r="F49" s="85"/>
-      <c r="G49" s="85"/>
-      <c r="H49" s="85"/>
-      <c r="I49" s="85"/>
-      <c r="J49" s="85"/>
-      <c r="K49" s="85"/>
-      <c r="L49" s="86"/>
-      <c r="M49" s="94">
+      <c r="B49" s="83"/>
+      <c r="C49" s="84"/>
+      <c r="D49" s="84"/>
+      <c r="E49" s="84"/>
+      <c r="F49" s="84"/>
+      <c r="G49" s="84"/>
+      <c r="H49" s="84"/>
+      <c r="I49" s="84"/>
+      <c r="J49" s="84"/>
+      <c r="K49" s="84"/>
+      <c r="L49" s="85"/>
+      <c r="M49" s="93">
         <v>5</v>
       </c>
       <c r="N49" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="S49" s="127"/>
-      <c r="T49" s="127"/>
-      <c r="U49" s="127"/>
+      <c r="S49" s="124"/>
+      <c r="T49" s="124"/>
+      <c r="U49" s="124"/>
       <c r="V49" s="71"/>
-      <c r="X49" s="128"/>
-      <c r="Y49" s="128"/>
-      <c r="Z49" s="128"/>
-      <c r="AA49" s="128"/>
-      <c r="AB49" s="128"/>
-      <c r="AC49" s="128"/>
-      <c r="AD49" s="128"/>
-      <c r="AE49" s="128"/>
+      <c r="X49" s="125"/>
+      <c r="Y49" s="125"/>
+      <c r="Z49" s="125"/>
+      <c r="AA49" s="125"/>
+      <c r="AB49" s="125"/>
+      <c r="AC49" s="125"/>
+      <c r="AD49" s="125"/>
+      <c r="AE49" s="125"/>
       <c r="AF49" s="44"/>
     </row>
     <row r="50" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="96" t="s">
+      <c r="B50" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="C50" s="97"/>
-      <c r="D50" s="97"/>
-      <c r="E50" s="97" t="s">
+      <c r="C50" s="96"/>
+      <c r="D50" s="96"/>
+      <c r="E50" s="96" t="s">
         <v>70</v>
       </c>
-      <c r="F50" s="97"/>
-      <c r="G50" s="97"/>
-      <c r="H50" s="97"/>
-      <c r="I50" s="97"/>
-      <c r="J50" s="97"/>
-      <c r="K50" s="97"/>
-      <c r="L50" s="98"/>
-      <c r="M50" s="84"/>
-      <c r="N50" s="85"/>
-      <c r="O50" s="85"/>
-      <c r="P50" s="85"/>
-      <c r="Q50" s="85"/>
-      <c r="R50" s="85"/>
-      <c r="S50" s="85"/>
-      <c r="T50" s="85"/>
-      <c r="U50" s="85"/>
-      <c r="V50" s="85"/>
-      <c r="W50" s="85"/>
-      <c r="X50" s="85"/>
-      <c r="Y50" s="85"/>
-      <c r="Z50" s="85"/>
-      <c r="AA50" s="85"/>
-      <c r="AB50" s="85"/>
-      <c r="AC50" s="85"/>
-      <c r="AD50" s="85"/>
-      <c r="AE50" s="85"/>
-      <c r="AF50" s="86"/>
+      <c r="F50" s="96"/>
+      <c r="G50" s="96"/>
+      <c r="H50" s="96"/>
+      <c r="I50" s="96"/>
+      <c r="J50" s="96"/>
+      <c r="K50" s="96"/>
+      <c r="L50" s="97"/>
+      <c r="M50" s="83"/>
+      <c r="N50" s="84"/>
+      <c r="O50" s="84"/>
+      <c r="P50" s="84"/>
+      <c r="Q50" s="84"/>
+      <c r="R50" s="84"/>
+      <c r="S50" s="84"/>
+      <c r="T50" s="84"/>
+      <c r="U50" s="84"/>
+      <c r="V50" s="84"/>
+      <c r="W50" s="84"/>
+      <c r="X50" s="84"/>
+      <c r="Y50" s="84"/>
+      <c r="Z50" s="84"/>
+      <c r="AA50" s="84"/>
+      <c r="AB50" s="84"/>
+      <c r="AC50" s="84"/>
+      <c r="AD50" s="84"/>
+      <c r="AE50" s="84"/>
+      <c r="AF50" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="67">
@@ -5846,8 +5842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A9:X42"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6828,58 +6824,58 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="183" t="s">
+      <c r="B10" s="181" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="184"/>
-      <c r="D10" s="184"/>
-      <c r="E10" s="184"/>
-      <c r="F10" s="184"/>
-      <c r="G10" s="184"/>
-      <c r="H10" s="184"/>
-      <c r="I10" s="184"/>
-      <c r="J10" s="184"/>
-      <c r="K10" s="184"/>
-      <c r="L10" s="184"/>
-      <c r="M10" s="184"/>
-      <c r="N10" s="184"/>
-      <c r="O10" s="184"/>
-      <c r="P10" s="184"/>
-      <c r="Q10" s="184"/>
-      <c r="R10" s="184"/>
-      <c r="S10" s="184"/>
-      <c r="T10" s="184"/>
-      <c r="U10" s="101"/>
-      <c r="V10" s="102"/>
-      <c r="W10" s="185" t="s">
+      <c r="C10" s="182"/>
+      <c r="D10" s="182"/>
+      <c r="E10" s="182"/>
+      <c r="F10" s="182"/>
+      <c r="G10" s="182"/>
+      <c r="H10" s="182"/>
+      <c r="I10" s="182"/>
+      <c r="J10" s="182"/>
+      <c r="K10" s="182"/>
+      <c r="L10" s="182"/>
+      <c r="M10" s="182"/>
+      <c r="N10" s="182"/>
+      <c r="O10" s="182"/>
+      <c r="P10" s="182"/>
+      <c r="Q10" s="182"/>
+      <c r="R10" s="182"/>
+      <c r="S10" s="182"/>
+      <c r="T10" s="182"/>
+      <c r="U10" s="100"/>
+      <c r="V10" s="101"/>
+      <c r="W10" s="183" t="s">
         <v>72</v>
       </c>
-      <c r="X10" s="186"/>
+      <c r="X10" s="184"/>
     </row>
     <row r="11" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="103"/>
-      <c r="C11" s="189"/>
-      <c r="D11" s="189"/>
-      <c r="E11" s="189"/>
-      <c r="F11" s="189"/>
-      <c r="G11" s="104"/>
-      <c r="H11" s="104"/>
-      <c r="I11" s="189"/>
-      <c r="J11" s="189"/>
-      <c r="K11" s="105"/>
-      <c r="L11" s="106"/>
-      <c r="M11" s="106"/>
-      <c r="N11" s="105"/>
-      <c r="O11" s="106"/>
-      <c r="P11" s="105"/>
-      <c r="Q11" s="85"/>
-      <c r="R11" s="85"/>
-      <c r="S11" s="85"/>
-      <c r="T11" s="85"/>
-      <c r="U11" s="85"/>
-      <c r="V11" s="107"/>
-      <c r="W11" s="187"/>
-      <c r="X11" s="188"/>
+      <c r="B11" s="102"/>
+      <c r="C11" s="187"/>
+      <c r="D11" s="187"/>
+      <c r="E11" s="187"/>
+      <c r="F11" s="187"/>
+      <c r="G11" s="103"/>
+      <c r="H11" s="103"/>
+      <c r="I11" s="187"/>
+      <c r="J11" s="187"/>
+      <c r="K11" s="104"/>
+      <c r="L11" s="105"/>
+      <c r="M11" s="105"/>
+      <c r="N11" s="104"/>
+      <c r="O11" s="105"/>
+      <c r="P11" s="104"/>
+      <c r="Q11" s="84"/>
+      <c r="R11" s="84"/>
+      <c r="S11" s="84"/>
+      <c r="T11" s="84"/>
+      <c r="U11" s="84"/>
+      <c r="V11" s="106"/>
+      <c r="W11" s="185"/>
+      <c r="X11" s="186"/>
     </row>
     <row r="12" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="64" t="s">
@@ -6922,28 +6918,28 @@
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
-      <c r="K13" s="190" t="s">
+      <c r="K13" s="188" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="190"/>
+      <c r="L13" s="188"/>
       <c r="M13" s="31"/>
       <c r="N13" s="27"/>
       <c r="O13" s="28"/>
       <c r="P13" s="28"/>
-      <c r="Q13" s="93" t="s">
+      <c r="Q13" s="92" t="s">
         <v>76</v>
       </c>
-      <c r="R13" s="93"/>
-      <c r="S13" s="190" t="s">
+      <c r="R13" s="92"/>
+      <c r="S13" s="188" t="s">
         <v>77</v>
       </c>
-      <c r="T13" s="190"/>
+      <c r="T13" s="188"/>
       <c r="U13" s="29"/>
-      <c r="V13" s="134" t="s">
+      <c r="V13" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="W13" s="134"/>
-      <c r="X13" s="108"/>
+      <c r="W13" s="131"/>
+      <c r="X13" s="107"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="27">
@@ -6953,7 +6949,7 @@
         <v>78</v>
       </c>
       <c r="D14" s="28"/>
-      <c r="E14" s="122"/>
+      <c r="E14" s="118"/>
       <c r="F14" s="28" t="s">
         <v>79</v>
       </c>
@@ -6968,24 +6964,24 @@
       <c r="N14" s="27"/>
       <c r="O14" s="28"/>
       <c r="P14" s="28"/>
-      <c r="Q14" s="109" t="s">
+      <c r="Q14" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="R14" s="93"/>
-      <c r="S14" s="191" t="s">
+      <c r="R14" s="92"/>
+      <c r="S14" s="189" t="s">
         <v>80</v>
       </c>
-      <c r="T14" s="191"/>
+      <c r="T14" s="189"/>
       <c r="U14" s="29"/>
-      <c r="V14" s="134"/>
-      <c r="W14" s="134"/>
-      <c r="X14" s="108"/>
+      <c r="V14" s="131"/>
+      <c r="W14" s="131"/>
+      <c r="X14" s="107"/>
     </row>
     <row r="15" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="27"/>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
-      <c r="E15" s="122"/>
+      <c r="E15" s="118"/>
       <c r="F15" s="28" t="s">
         <v>81</v>
       </c>
@@ -7006,18 +7002,18 @@
       <c r="P15" s="28"/>
       <c r="Q15" s="31"/>
       <c r="R15" s="28"/>
-      <c r="S15" s="119"/>
-      <c r="T15" s="45"/>
+      <c r="S15" s="177"/>
+      <c r="T15" s="177"/>
       <c r="U15" s="28"/>
-      <c r="V15" s="121"/>
-      <c r="W15" s="45"/>
+      <c r="V15" s="177"/>
+      <c r="W15" s="177"/>
       <c r="X15" s="55"/>
     </row>
     <row r="16" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="27"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
-      <c r="E16" s="122"/>
+      <c r="E16" s="118"/>
       <c r="F16" s="28" t="s">
         <v>83</v>
       </c>
@@ -7031,14 +7027,14 @@
       <c r="M16" s="28"/>
       <c r="N16" s="70"/>
       <c r="S16" s="51"/>
-      <c r="V16" s="123"/>
+      <c r="V16" s="119"/>
       <c r="X16" s="44"/>
     </row>
     <row r="17" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="27"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
-      <c r="E17" s="122"/>
+      <c r="E17" s="118"/>
       <c r="F17" s="28" t="s">
         <v>84</v>
       </c>
@@ -7057,18 +7053,18 @@
       <c r="P17" s="28"/>
       <c r="Q17" s="31"/>
       <c r="R17" s="28"/>
-      <c r="S17" s="119"/>
-      <c r="T17" s="45"/>
+      <c r="S17" s="177"/>
+      <c r="T17" s="177"/>
       <c r="U17" s="28"/>
-      <c r="V17" s="121"/>
-      <c r="W17" s="45"/>
+      <c r="V17" s="177"/>
+      <c r="W17" s="177"/>
       <c r="X17" s="55"/>
     </row>
     <row r="18" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="27"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
-      <c r="E18" s="122"/>
+      <c r="E18" s="118"/>
       <c r="F18" s="28" t="s">
         <v>86</v>
       </c>
@@ -7080,7 +7076,7 @@
       <c r="M18" s="28"/>
       <c r="N18" s="70"/>
       <c r="S18" s="51"/>
-      <c r="V18" s="123"/>
+      <c r="V18" s="119"/>
       <c r="X18" s="44"/>
     </row>
     <row r="19" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7091,7 +7087,7 @@
         <v>87</v>
       </c>
       <c r="D19" s="28"/>
-      <c r="E19" s="122"/>
+      <c r="E19" s="118"/>
       <c r="F19" s="28" t="s">
         <v>88</v>
       </c>
@@ -7110,18 +7106,18 @@
       <c r="P19" s="28"/>
       <c r="Q19" s="31"/>
       <c r="R19" s="28"/>
-      <c r="S19" s="119"/>
-      <c r="T19" s="45"/>
+      <c r="S19" s="177"/>
+      <c r="T19" s="177"/>
       <c r="U19" s="28"/>
-      <c r="V19" s="121"/>
-      <c r="W19" s="45"/>
+      <c r="V19" s="177"/>
+      <c r="W19" s="177"/>
       <c r="X19" s="55"/>
     </row>
     <row r="20" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="27"/>
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
-      <c r="E20" s="122"/>
+      <c r="E20" s="118"/>
       <c r="F20" s="28" t="s">
         <v>90</v>
       </c>
@@ -7136,10 +7132,10 @@
       <c r="P20" s="28"/>
       <c r="Q20" s="28"/>
       <c r="R20" s="28"/>
-      <c r="S20" s="120"/>
+      <c r="S20" s="117"/>
       <c r="T20" s="28"/>
       <c r="U20" s="28"/>
-      <c r="V20" s="124"/>
+      <c r="V20" s="120"/>
       <c r="W20" s="28"/>
       <c r="X20" s="55"/>
     </row>
@@ -7151,7 +7147,7 @@
         <v>91</v>
       </c>
       <c r="D21" s="28"/>
-      <c r="E21" s="122"/>
+      <c r="E21" s="118"/>
       <c r="F21" s="28" t="s">
         <v>92</v>
       </c>
@@ -7170,18 +7166,18 @@
       <c r="P21" s="28"/>
       <c r="Q21" s="31"/>
       <c r="R21" s="28"/>
-      <c r="S21" s="119"/>
-      <c r="T21" s="45"/>
+      <c r="S21" s="177"/>
+      <c r="T21" s="177"/>
       <c r="U21" s="28"/>
-      <c r="V21" s="121"/>
-      <c r="W21" s="45"/>
+      <c r="V21" s="177"/>
+      <c r="W21" s="177"/>
       <c r="X21" s="55"/>
     </row>
     <row r="22" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="27"/>
       <c r="C22" s="28"/>
       <c r="D22" s="28"/>
-      <c r="E22" s="122"/>
+      <c r="E22" s="118"/>
       <c r="F22" s="28" t="s">
         <v>94</v>
       </c>
@@ -7193,14 +7189,14 @@
       <c r="M22" s="28"/>
       <c r="N22" s="70"/>
       <c r="S22" s="51"/>
-      <c r="V22" s="124"/>
+      <c r="V22" s="120"/>
       <c r="X22" s="44"/>
     </row>
     <row r="23" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
       <c r="D23" s="28"/>
-      <c r="E23" s="122"/>
+      <c r="E23" s="118"/>
       <c r="F23" s="28" t="s">
         <v>95</v>
       </c>
@@ -7219,11 +7215,11 @@
       <c r="P23" s="28"/>
       <c r="Q23" s="31"/>
       <c r="R23" s="28"/>
-      <c r="S23" s="119"/>
-      <c r="T23" s="45"/>
+      <c r="S23" s="177"/>
+      <c r="T23" s="177"/>
       <c r="U23" s="28"/>
-      <c r="V23" s="110"/>
-      <c r="W23" s="45"/>
+      <c r="V23" s="177"/>
+      <c r="W23" s="177"/>
       <c r="X23" s="55"/>
     </row>
     <row r="24" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7240,46 +7236,46 @@
       <c r="L24" s="53"/>
       <c r="M24" s="28"/>
       <c r="N24" s="70"/>
-      <c r="P24" s="85"/>
-      <c r="Q24" s="85"/>
-      <c r="R24" s="85"/>
-      <c r="S24" s="85"/>
-      <c r="T24" s="85"/>
-      <c r="U24" s="85"/>
-      <c r="V24" s="111"/>
-      <c r="W24" s="85"/>
-      <c r="X24" s="86"/>
+      <c r="P24" s="84"/>
+      <c r="Q24" s="84"/>
+      <c r="R24" s="84"/>
+      <c r="S24" s="84"/>
+      <c r="T24" s="84"/>
+      <c r="U24" s="84"/>
+      <c r="V24" s="109"/>
+      <c r="W24" s="84"/>
+      <c r="X24" s="85"/>
     </row>
     <row r="25" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="192" t="s">
+      <c r="B25" s="190" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="193"/>
-      <c r="D25" s="193"/>
-      <c r="E25" s="193"/>
-      <c r="F25" s="193"/>
-      <c r="G25" s="193"/>
-      <c r="H25" s="193"/>
-      <c r="I25" s="193"/>
-      <c r="J25" s="193"/>
-      <c r="K25" s="193"/>
-      <c r="L25" s="193"/>
-      <c r="M25" s="193"/>
-      <c r="N25" s="193"/>
-      <c r="O25" s="193"/>
-      <c r="P25" s="192" t="s">
+      <c r="C25" s="191"/>
+      <c r="D25" s="191"/>
+      <c r="E25" s="191"/>
+      <c r="F25" s="191"/>
+      <c r="G25" s="191"/>
+      <c r="H25" s="191"/>
+      <c r="I25" s="191"/>
+      <c r="J25" s="191"/>
+      <c r="K25" s="191"/>
+      <c r="L25" s="191"/>
+      <c r="M25" s="191"/>
+      <c r="N25" s="191"/>
+      <c r="O25" s="191"/>
+      <c r="P25" s="190" t="s">
         <v>98</v>
       </c>
-      <c r="Q25" s="193"/>
-      <c r="R25" s="193"/>
-      <c r="S25" s="193"/>
-      <c r="T25" s="192" t="s">
+      <c r="Q25" s="191"/>
+      <c r="R25" s="191"/>
+      <c r="S25" s="191"/>
+      <c r="T25" s="190" t="s">
         <v>99</v>
       </c>
-      <c r="U25" s="193"/>
-      <c r="V25" s="193"/>
-      <c r="W25" s="193"/>
-      <c r="X25" s="194"/>
+      <c r="U25" s="191"/>
+      <c r="V25" s="191"/>
+      <c r="W25" s="191"/>
+      <c r="X25" s="192"/>
     </row>
     <row r="26" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="27">
@@ -7289,23 +7285,23 @@
         <v>100</v>
       </c>
       <c r="I26" s="39"/>
-      <c r="J26" s="112" t="s">
+      <c r="J26" s="110" t="s">
         <v>101</v>
       </c>
       <c r="K26" s="70"/>
-      <c r="P26" s="113" t="s">
+      <c r="P26" s="111" t="s">
         <v>102</v>
       </c>
-      <c r="Q26" s="127"/>
-      <c r="R26" s="127"/>
-      <c r="S26" s="127"/>
-      <c r="T26" s="113" t="s">
+      <c r="Q26" s="124"/>
+      <c r="R26" s="124"/>
+      <c r="S26" s="124"/>
+      <c r="T26" s="111" t="s">
         <v>102</v>
       </c>
-      <c r="U26" s="181"/>
-      <c r="V26" s="181"/>
-      <c r="W26" s="181"/>
-      <c r="X26" s="182"/>
+      <c r="U26" s="179"/>
+      <c r="V26" s="179"/>
+      <c r="W26" s="179"/>
+      <c r="X26" s="180"/>
     </row>
     <row r="27" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="27"/>
@@ -7313,23 +7309,23 @@
       <c r="D27" s="32">
         <v>1</v>
       </c>
-      <c r="E27" s="122"/>
-      <c r="F27" s="125" t="s">
+      <c r="E27" s="118"/>
+      <c r="F27" s="121" t="s">
         <v>112</v>
       </c>
       <c r="G27" s="39"/>
       <c r="H27" s="39"/>
       <c r="I27" s="39"/>
-      <c r="J27" s="114"/>
+      <c r="J27" s="112"/>
       <c r="K27" s="56"/>
-      <c r="M27" s="180"/>
-      <c r="N27" s="180"/>
+      <c r="M27" s="178"/>
+      <c r="N27" s="178"/>
       <c r="P27" s="70"/>
       <c r="T27" s="70"/>
-      <c r="U27" s="181"/>
-      <c r="V27" s="181"/>
-      <c r="W27" s="181"/>
-      <c r="X27" s="182"/>
+      <c r="U27" s="179"/>
+      <c r="V27" s="179"/>
+      <c r="W27" s="179"/>
+      <c r="X27" s="180"/>
     </row>
     <row r="28" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="27"/>
@@ -7337,32 +7333,32 @@
       <c r="D28" s="32">
         <v>2</v>
       </c>
-      <c r="E28" s="122"/>
-      <c r="F28" s="125" t="s">
+      <c r="E28" s="118"/>
+      <c r="F28" s="121" t="s">
         <v>113</v>
       </c>
       <c r="G28" s="39"/>
       <c r="H28" s="39"/>
       <c r="I28" s="39"/>
-      <c r="J28" s="115"/>
+      <c r="J28" s="113"/>
       <c r="K28" s="56"/>
       <c r="L28" s="28"/>
-      <c r="M28" s="180"/>
-      <c r="N28" s="180"/>
+      <c r="M28" s="178"/>
+      <c r="N28" s="178"/>
       <c r="O28" s="28"/>
-      <c r="P28" s="116" t="s">
+      <c r="P28" s="114" t="s">
         <v>103</v>
       </c>
-      <c r="Q28" s="127"/>
-      <c r="R28" s="127"/>
-      <c r="S28" s="127"/>
-      <c r="T28" s="116" t="s">
+      <c r="Q28" s="124"/>
+      <c r="R28" s="124"/>
+      <c r="S28" s="124"/>
+      <c r="T28" s="114" t="s">
         <v>103</v>
       </c>
-      <c r="U28" s="181"/>
-      <c r="V28" s="181"/>
-      <c r="W28" s="181"/>
-      <c r="X28" s="182"/>
+      <c r="U28" s="179"/>
+      <c r="V28" s="179"/>
+      <c r="W28" s="179"/>
+      <c r="X28" s="180"/>
     </row>
     <row r="29" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="27"/>
@@ -7370,32 +7366,32 @@
       <c r="D29" s="32">
         <v>3</v>
       </c>
-      <c r="E29" s="122"/>
-      <c r="F29" s="125" t="s">
+      <c r="E29" s="118"/>
+      <c r="F29" s="121" t="s">
         <v>114</v>
       </c>
       <c r="G29" s="39"/>
       <c r="H29" s="39"/>
       <c r="I29" s="39"/>
-      <c r="J29" s="115"/>
+      <c r="J29" s="113"/>
       <c r="K29" s="56"/>
       <c r="L29" s="28"/>
-      <c r="M29" s="180"/>
-      <c r="N29" s="180"/>
+      <c r="M29" s="178"/>
+      <c r="N29" s="178"/>
       <c r="O29" s="28"/>
-      <c r="P29" s="116" t="s">
+      <c r="P29" s="114" t="s">
         <v>104</v>
       </c>
-      <c r="Q29" s="127"/>
-      <c r="R29" s="127"/>
-      <c r="S29" s="127"/>
-      <c r="T29" s="116" t="s">
+      <c r="Q29" s="124"/>
+      <c r="R29" s="124"/>
+      <c r="S29" s="124"/>
+      <c r="T29" s="114" t="s">
         <v>104</v>
       </c>
-      <c r="U29" s="181"/>
-      <c r="V29" s="181"/>
-      <c r="W29" s="181"/>
-      <c r="X29" s="182"/>
+      <c r="U29" s="179"/>
+      <c r="V29" s="179"/>
+      <c r="W29" s="179"/>
+      <c r="X29" s="180"/>
     </row>
     <row r="30" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="27"/>
@@ -7405,33 +7401,33 @@
       <c r="F30" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="G30" s="122"/>
+      <c r="G30" s="118"/>
       <c r="H30" s="39" t="s">
         <v>116</v>
       </c>
       <c r="I30" s="39"/>
-      <c r="J30" s="115"/>
+      <c r="J30" s="113"/>
       <c r="K30" s="56"/>
       <c r="L30" s="28"/>
-      <c r="M30" s="180"/>
-      <c r="N30" s="180"/>
+      <c r="M30" s="178"/>
+      <c r="N30" s="178"/>
       <c r="O30" s="28"/>
-      <c r="P30" s="116" t="s">
+      <c r="P30" s="114" t="s">
         <v>105</v>
       </c>
-      <c r="Q30" s="202" t="s">
+      <c r="Q30" s="204" t="s">
         <v>106</v>
       </c>
-      <c r="R30" s="202"/>
-      <c r="S30" s="202"/>
-      <c r="T30" s="116" t="s">
+      <c r="R30" s="204"/>
+      <c r="S30" s="204"/>
+      <c r="T30" s="114" t="s">
         <v>105</v>
       </c>
-      <c r="V30" s="202" t="s">
+      <c r="V30" s="204" t="s">
         <v>106</v>
       </c>
-      <c r="W30" s="202"/>
-      <c r="X30" s="203"/>
+      <c r="W30" s="204"/>
+      <c r="X30" s="205"/>
     </row>
     <row r="31" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="27"/>
@@ -7439,30 +7435,30 @@
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
       <c r="F31" s="28"/>
-      <c r="G31" s="122"/>
+      <c r="G31" s="118"/>
       <c r="H31" s="39" t="s">
         <v>117</v>
       </c>
       <c r="I31" s="39"/>
-      <c r="J31" s="115"/>
+      <c r="J31" s="113"/>
       <c r="K31" s="56"/>
       <c r="L31" s="28"/>
-      <c r="M31" s="180"/>
-      <c r="N31" s="180"/>
+      <c r="M31" s="178"/>
+      <c r="N31" s="178"/>
       <c r="O31" s="28"/>
-      <c r="P31" s="116" t="s">
+      <c r="P31" s="114" t="s">
         <v>107</v>
       </c>
-      <c r="Q31" s="127"/>
-      <c r="R31" s="127"/>
-      <c r="S31" s="127"/>
-      <c r="T31" s="116" t="s">
+      <c r="Q31" s="124"/>
+      <c r="R31" s="124"/>
+      <c r="S31" s="124"/>
+      <c r="T31" s="114" t="s">
         <v>107</v>
       </c>
-      <c r="U31" s="181"/>
-      <c r="V31" s="181"/>
-      <c r="W31" s="181"/>
-      <c r="X31" s="182"/>
+      <c r="U31" s="179"/>
+      <c r="V31" s="179"/>
+      <c r="W31" s="179"/>
+      <c r="X31" s="180"/>
     </row>
     <row r="32" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="59"/>
@@ -7470,287 +7466,307 @@
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
-      <c r="G32" s="122"/>
+      <c r="G32" s="118"/>
       <c r="H32" s="39" t="s">
         <v>118</v>
       </c>
       <c r="I32" s="60"/>
-      <c r="J32" s="117"/>
-      <c r="K32" s="85"/>
+      <c r="J32" s="115"/>
+      <c r="K32" s="84"/>
       <c r="L32" s="60"/>
       <c r="M32" s="60"/>
       <c r="N32" s="60"/>
       <c r="O32" s="61"/>
-      <c r="P32" s="118" t="s">
+      <c r="P32" s="116" t="s">
         <v>108</v>
       </c>
-      <c r="Q32" s="204" t="s">
+      <c r="Q32" s="193" t="s">
         <v>109</v>
       </c>
-      <c r="R32" s="205"/>
-      <c r="S32" s="204" t="s">
+      <c r="R32" s="194"/>
+      <c r="S32" s="193" t="s">
         <v>110</v>
       </c>
-      <c r="T32" s="206"/>
-      <c r="U32" s="206"/>
-      <c r="V32" s="206"/>
-      <c r="W32" s="206"/>
-      <c r="X32" s="207"/>
+      <c r="T32" s="195"/>
+      <c r="U32" s="195"/>
+      <c r="V32" s="195"/>
+      <c r="W32" s="195"/>
+      <c r="X32" s="196"/>
     </row>
     <row r="33" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="192" t="s">
+      <c r="B33" s="190" t="s">
         <v>111</v>
       </c>
-      <c r="C33" s="193"/>
-      <c r="D33" s="193"/>
-      <c r="E33" s="193"/>
-      <c r="F33" s="193"/>
-      <c r="G33" s="193"/>
-      <c r="H33" s="193"/>
-      <c r="I33" s="193"/>
-      <c r="J33" s="193"/>
-      <c r="K33" s="193"/>
-      <c r="L33" s="193"/>
-      <c r="M33" s="193"/>
-      <c r="N33" s="193"/>
-      <c r="O33" s="194"/>
-      <c r="P33" s="199"/>
-      <c r="Q33" s="195"/>
-      <c r="R33" s="200"/>
-      <c r="S33" s="195"/>
-      <c r="T33" s="132"/>
-      <c r="U33" s="132"/>
-      <c r="V33" s="132"/>
-      <c r="W33" s="132"/>
-      <c r="X33" s="196"/>
+      <c r="C33" s="191"/>
+      <c r="D33" s="191"/>
+      <c r="E33" s="191"/>
+      <c r="F33" s="191"/>
+      <c r="G33" s="191"/>
+      <c r="H33" s="191"/>
+      <c r="I33" s="191"/>
+      <c r="J33" s="191"/>
+      <c r="K33" s="191"/>
+      <c r="L33" s="191"/>
+      <c r="M33" s="191"/>
+      <c r="N33" s="191"/>
+      <c r="O33" s="192"/>
+      <c r="P33" s="197"/>
+      <c r="Q33" s="198"/>
+      <c r="R33" s="199"/>
+      <c r="S33" s="198"/>
+      <c r="T33" s="129"/>
+      <c r="U33" s="129"/>
+      <c r="V33" s="129"/>
+      <c r="W33" s="129"/>
+      <c r="X33" s="202"/>
     </row>
     <row r="34" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="208"/>
-      <c r="C34" s="209"/>
-      <c r="D34" s="209"/>
-      <c r="E34" s="209"/>
-      <c r="F34" s="209"/>
-      <c r="G34" s="209"/>
-      <c r="H34" s="209"/>
-      <c r="I34" s="209"/>
-      <c r="J34" s="209"/>
-      <c r="K34" s="209"/>
-      <c r="L34" s="209"/>
-      <c r="M34" s="209"/>
-      <c r="N34" s="209"/>
-      <c r="O34" s="210"/>
-      <c r="P34" s="199"/>
-      <c r="Q34" s="197"/>
+      <c r="B34" s="206"/>
+      <c r="C34" s="207"/>
+      <c r="D34" s="207"/>
+      <c r="E34" s="207"/>
+      <c r="F34" s="207"/>
+      <c r="G34" s="207"/>
+      <c r="H34" s="207"/>
+      <c r="I34" s="207"/>
+      <c r="J34" s="207"/>
+      <c r="K34" s="207"/>
+      <c r="L34" s="207"/>
+      <c r="M34" s="207"/>
+      <c r="N34" s="207"/>
+      <c r="O34" s="208"/>
+      <c r="P34" s="197"/>
+      <c r="Q34" s="200"/>
       <c r="R34" s="201"/>
-      <c r="S34" s="197"/>
-      <c r="T34" s="130"/>
-      <c r="U34" s="130"/>
-      <c r="V34" s="130"/>
-      <c r="W34" s="130"/>
-      <c r="X34" s="198"/>
+      <c r="S34" s="200"/>
+      <c r="T34" s="127"/>
+      <c r="U34" s="127"/>
+      <c r="V34" s="127"/>
+      <c r="W34" s="127"/>
+      <c r="X34" s="203"/>
     </row>
     <row r="35" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="208"/>
-      <c r="C35" s="209"/>
-      <c r="D35" s="209"/>
-      <c r="E35" s="209"/>
-      <c r="F35" s="209"/>
-      <c r="G35" s="209"/>
-      <c r="H35" s="209"/>
-      <c r="I35" s="209"/>
-      <c r="J35" s="209"/>
-      <c r="K35" s="209"/>
-      <c r="L35" s="209"/>
-      <c r="M35" s="209"/>
-      <c r="N35" s="209"/>
-      <c r="O35" s="210"/>
-      <c r="P35" s="199"/>
-      <c r="Q35" s="195"/>
-      <c r="R35" s="200"/>
-      <c r="S35" s="195"/>
-      <c r="T35" s="132"/>
-      <c r="U35" s="132"/>
-      <c r="V35" s="132"/>
-      <c r="W35" s="132"/>
-      <c r="X35" s="196"/>
+      <c r="B35" s="206"/>
+      <c r="C35" s="207"/>
+      <c r="D35" s="207"/>
+      <c r="E35" s="207"/>
+      <c r="F35" s="207"/>
+      <c r="G35" s="207"/>
+      <c r="H35" s="207"/>
+      <c r="I35" s="207"/>
+      <c r="J35" s="207"/>
+      <c r="K35" s="207"/>
+      <c r="L35" s="207"/>
+      <c r="M35" s="207"/>
+      <c r="N35" s="207"/>
+      <c r="O35" s="208"/>
+      <c r="P35" s="197"/>
+      <c r="Q35" s="198"/>
+      <c r="R35" s="199"/>
+      <c r="S35" s="198"/>
+      <c r="T35" s="129"/>
+      <c r="U35" s="129"/>
+      <c r="V35" s="129"/>
+      <c r="W35" s="129"/>
+      <c r="X35" s="202"/>
     </row>
     <row r="36" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="208"/>
-      <c r="C36" s="209"/>
-      <c r="D36" s="209"/>
-      <c r="E36" s="209"/>
-      <c r="F36" s="209"/>
-      <c r="G36" s="209"/>
-      <c r="H36" s="209"/>
-      <c r="I36" s="209"/>
-      <c r="J36" s="209"/>
-      <c r="K36" s="209"/>
-      <c r="L36" s="209"/>
-      <c r="M36" s="209"/>
-      <c r="N36" s="209"/>
-      <c r="O36" s="210"/>
-      <c r="P36" s="199"/>
-      <c r="Q36" s="197"/>
+      <c r="B36" s="206"/>
+      <c r="C36" s="207"/>
+      <c r="D36" s="207"/>
+      <c r="E36" s="207"/>
+      <c r="F36" s="207"/>
+      <c r="G36" s="207"/>
+      <c r="H36" s="207"/>
+      <c r="I36" s="207"/>
+      <c r="J36" s="207"/>
+      <c r="K36" s="207"/>
+      <c r="L36" s="207"/>
+      <c r="M36" s="207"/>
+      <c r="N36" s="207"/>
+      <c r="O36" s="208"/>
+      <c r="P36" s="197"/>
+      <c r="Q36" s="200"/>
       <c r="R36" s="201"/>
-      <c r="S36" s="197"/>
-      <c r="T36" s="130"/>
-      <c r="U36" s="130"/>
-      <c r="V36" s="130"/>
-      <c r="W36" s="130"/>
-      <c r="X36" s="198"/>
+      <c r="S36" s="200"/>
+      <c r="T36" s="127"/>
+      <c r="U36" s="127"/>
+      <c r="V36" s="127"/>
+      <c r="W36" s="127"/>
+      <c r="X36" s="203"/>
     </row>
     <row r="37" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="208"/>
-      <c r="C37" s="209"/>
-      <c r="D37" s="209"/>
-      <c r="E37" s="209"/>
-      <c r="F37" s="209"/>
-      <c r="G37" s="209"/>
-      <c r="H37" s="209"/>
-      <c r="I37" s="209"/>
-      <c r="J37" s="209"/>
-      <c r="K37" s="209"/>
-      <c r="L37" s="209"/>
-      <c r="M37" s="209"/>
-      <c r="N37" s="209"/>
-      <c r="O37" s="210"/>
-      <c r="P37" s="199"/>
-      <c r="Q37" s="195"/>
-      <c r="R37" s="200"/>
-      <c r="S37" s="195"/>
-      <c r="T37" s="132"/>
-      <c r="U37" s="132"/>
-      <c r="V37" s="132"/>
-      <c r="W37" s="132"/>
-      <c r="X37" s="196"/>
+      <c r="B37" s="206"/>
+      <c r="C37" s="207"/>
+      <c r="D37" s="207"/>
+      <c r="E37" s="207"/>
+      <c r="F37" s="207"/>
+      <c r="G37" s="207"/>
+      <c r="H37" s="207"/>
+      <c r="I37" s="207"/>
+      <c r="J37" s="207"/>
+      <c r="K37" s="207"/>
+      <c r="L37" s="207"/>
+      <c r="M37" s="207"/>
+      <c r="N37" s="207"/>
+      <c r="O37" s="208"/>
+      <c r="P37" s="197"/>
+      <c r="Q37" s="198"/>
+      <c r="R37" s="199"/>
+      <c r="S37" s="198"/>
+      <c r="T37" s="129"/>
+      <c r="U37" s="129"/>
+      <c r="V37" s="129"/>
+      <c r="W37" s="129"/>
+      <c r="X37" s="202"/>
     </row>
     <row r="38" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="208"/>
-      <c r="C38" s="209"/>
-      <c r="D38" s="209"/>
-      <c r="E38" s="209"/>
-      <c r="F38" s="209"/>
-      <c r="G38" s="209"/>
-      <c r="H38" s="209"/>
-      <c r="I38" s="209"/>
-      <c r="J38" s="209"/>
-      <c r="K38" s="209"/>
-      <c r="L38" s="209"/>
-      <c r="M38" s="209"/>
-      <c r="N38" s="209"/>
-      <c r="O38" s="210"/>
-      <c r="P38" s="199"/>
-      <c r="Q38" s="197"/>
+      <c r="B38" s="206"/>
+      <c r="C38" s="207"/>
+      <c r="D38" s="207"/>
+      <c r="E38" s="207"/>
+      <c r="F38" s="207"/>
+      <c r="G38" s="207"/>
+      <c r="H38" s="207"/>
+      <c r="I38" s="207"/>
+      <c r="J38" s="207"/>
+      <c r="K38" s="207"/>
+      <c r="L38" s="207"/>
+      <c r="M38" s="207"/>
+      <c r="N38" s="207"/>
+      <c r="O38" s="208"/>
+      <c r="P38" s="197"/>
+      <c r="Q38" s="200"/>
       <c r="R38" s="201"/>
-      <c r="S38" s="197"/>
-      <c r="T38" s="130"/>
-      <c r="U38" s="130"/>
-      <c r="V38" s="130"/>
-      <c r="W38" s="130"/>
-      <c r="X38" s="198"/>
+      <c r="S38" s="200"/>
+      <c r="T38" s="127"/>
+      <c r="U38" s="127"/>
+      <c r="V38" s="127"/>
+      <c r="W38" s="127"/>
+      <c r="X38" s="203"/>
     </row>
     <row r="39" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="208"/>
-      <c r="C39" s="209"/>
-      <c r="D39" s="209"/>
-      <c r="E39" s="209"/>
-      <c r="F39" s="209"/>
-      <c r="G39" s="209"/>
-      <c r="H39" s="209"/>
-      <c r="I39" s="209"/>
-      <c r="J39" s="209"/>
-      <c r="K39" s="209"/>
-      <c r="L39" s="209"/>
-      <c r="M39" s="209"/>
-      <c r="N39" s="209"/>
-      <c r="O39" s="210"/>
-      <c r="P39" s="199"/>
-      <c r="Q39" s="195"/>
-      <c r="R39" s="200"/>
-      <c r="S39" s="195"/>
-      <c r="T39" s="132"/>
-      <c r="U39" s="132"/>
-      <c r="V39" s="132"/>
-      <c r="W39" s="132"/>
-      <c r="X39" s="196"/>
+      <c r="B39" s="206"/>
+      <c r="C39" s="207"/>
+      <c r="D39" s="207"/>
+      <c r="E39" s="207"/>
+      <c r="F39" s="207"/>
+      <c r="G39" s="207"/>
+      <c r="H39" s="207"/>
+      <c r="I39" s="207"/>
+      <c r="J39" s="207"/>
+      <c r="K39" s="207"/>
+      <c r="L39" s="207"/>
+      <c r="M39" s="207"/>
+      <c r="N39" s="207"/>
+      <c r="O39" s="208"/>
+      <c r="P39" s="197"/>
+      <c r="Q39" s="198"/>
+      <c r="R39" s="199"/>
+      <c r="S39" s="198"/>
+      <c r="T39" s="129"/>
+      <c r="U39" s="129"/>
+      <c r="V39" s="129"/>
+      <c r="W39" s="129"/>
+      <c r="X39" s="202"/>
     </row>
     <row r="40" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="208"/>
-      <c r="C40" s="209"/>
-      <c r="D40" s="209"/>
-      <c r="E40" s="209"/>
-      <c r="F40" s="209"/>
-      <c r="G40" s="209"/>
-      <c r="H40" s="209"/>
-      <c r="I40" s="209"/>
-      <c r="J40" s="209"/>
-      <c r="K40" s="209"/>
-      <c r="L40" s="209"/>
-      <c r="M40" s="209"/>
-      <c r="N40" s="209"/>
-      <c r="O40" s="210"/>
-      <c r="P40" s="199"/>
-      <c r="Q40" s="197"/>
+      <c r="B40" s="206"/>
+      <c r="C40" s="207"/>
+      <c r="D40" s="207"/>
+      <c r="E40" s="207"/>
+      <c r="F40" s="207"/>
+      <c r="G40" s="207"/>
+      <c r="H40" s="207"/>
+      <c r="I40" s="207"/>
+      <c r="J40" s="207"/>
+      <c r="K40" s="207"/>
+      <c r="L40" s="207"/>
+      <c r="M40" s="207"/>
+      <c r="N40" s="207"/>
+      <c r="O40" s="208"/>
+      <c r="P40" s="197"/>
+      <c r="Q40" s="200"/>
       <c r="R40" s="201"/>
-      <c r="S40" s="197"/>
-      <c r="T40" s="130"/>
-      <c r="U40" s="130"/>
-      <c r="V40" s="130"/>
-      <c r="W40" s="130"/>
-      <c r="X40" s="198"/>
+      <c r="S40" s="200"/>
+      <c r="T40" s="127"/>
+      <c r="U40" s="127"/>
+      <c r="V40" s="127"/>
+      <c r="W40" s="127"/>
+      <c r="X40" s="203"/>
     </row>
     <row r="41" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="208"/>
-      <c r="C41" s="209"/>
-      <c r="D41" s="209"/>
-      <c r="E41" s="209"/>
-      <c r="F41" s="209"/>
-      <c r="G41" s="209"/>
-      <c r="H41" s="209"/>
-      <c r="I41" s="209"/>
-      <c r="J41" s="209"/>
-      <c r="K41" s="209"/>
-      <c r="L41" s="209"/>
-      <c r="M41" s="209"/>
-      <c r="N41" s="209"/>
-      <c r="O41" s="210"/>
-      <c r="P41" s="199"/>
-      <c r="Q41" s="195"/>
-      <c r="R41" s="200"/>
-      <c r="S41" s="195"/>
-      <c r="T41" s="132"/>
-      <c r="U41" s="132"/>
-      <c r="V41" s="132"/>
-      <c r="W41" s="132"/>
-      <c r="X41" s="196"/>
+      <c r="B41" s="206"/>
+      <c r="C41" s="207"/>
+      <c r="D41" s="207"/>
+      <c r="E41" s="207"/>
+      <c r="F41" s="207"/>
+      <c r="G41" s="207"/>
+      <c r="H41" s="207"/>
+      <c r="I41" s="207"/>
+      <c r="J41" s="207"/>
+      <c r="K41" s="207"/>
+      <c r="L41" s="207"/>
+      <c r="M41" s="207"/>
+      <c r="N41" s="207"/>
+      <c r="O41" s="208"/>
+      <c r="P41" s="197"/>
+      <c r="Q41" s="198"/>
+      <c r="R41" s="199"/>
+      <c r="S41" s="198"/>
+      <c r="T41" s="129"/>
+      <c r="U41" s="129"/>
+      <c r="V41" s="129"/>
+      <c r="W41" s="129"/>
+      <c r="X41" s="202"/>
     </row>
     <row r="42" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="211"/>
-      <c r="C42" s="212"/>
-      <c r="D42" s="212"/>
-      <c r="E42" s="212"/>
-      <c r="F42" s="212"/>
-      <c r="G42" s="212"/>
-      <c r="H42" s="212"/>
-      <c r="I42" s="212"/>
-      <c r="J42" s="212"/>
-      <c r="K42" s="212"/>
-      <c r="L42" s="212"/>
-      <c r="M42" s="212"/>
-      <c r="N42" s="212"/>
-      <c r="O42" s="213"/>
-      <c r="P42" s="214"/>
-      <c r="Q42" s="215"/>
-      <c r="R42" s="216"/>
-      <c r="S42" s="215"/>
-      <c r="T42" s="217"/>
-      <c r="U42" s="217"/>
-      <c r="V42" s="217"/>
-      <c r="W42" s="217"/>
-      <c r="X42" s="218"/>
+      <c r="B42" s="209"/>
+      <c r="C42" s="210"/>
+      <c r="D42" s="210"/>
+      <c r="E42" s="210"/>
+      <c r="F42" s="210"/>
+      <c r="G42" s="210"/>
+      <c r="H42" s="210"/>
+      <c r="I42" s="210"/>
+      <c r="J42" s="210"/>
+      <c r="K42" s="210"/>
+      <c r="L42" s="210"/>
+      <c r="M42" s="210"/>
+      <c r="N42" s="210"/>
+      <c r="O42" s="211"/>
+      <c r="P42" s="212"/>
+      <c r="Q42" s="213"/>
+      <c r="R42" s="214"/>
+      <c r="S42" s="213"/>
+      <c r="T42" s="215"/>
+      <c r="U42" s="215"/>
+      <c r="V42" s="215"/>
+      <c r="W42" s="215"/>
+      <c r="X42" s="216"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="56">
+    <mergeCell ref="P39:P40"/>
+    <mergeCell ref="Q39:R40"/>
+    <mergeCell ref="S39:X40"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="Q30:S30"/>
+    <mergeCell ref="V30:X30"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="Q31:S31"/>
+    <mergeCell ref="U31:X31"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="S32:X32"/>
+    <mergeCell ref="B33:O33"/>
+    <mergeCell ref="P33:P34"/>
+    <mergeCell ref="Q33:R34"/>
+    <mergeCell ref="S33:X34"/>
     <mergeCell ref="B34:O42"/>
     <mergeCell ref="P35:P36"/>
     <mergeCell ref="Q35:R36"/>
@@ -7761,29 +7777,13 @@
     <mergeCell ref="P37:P38"/>
     <mergeCell ref="Q37:R38"/>
     <mergeCell ref="S37:X38"/>
-    <mergeCell ref="P39:P40"/>
-    <mergeCell ref="Q39:R40"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="Q30:S30"/>
-    <mergeCell ref="V30:X30"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="Q31:S31"/>
-    <mergeCell ref="U31:X31"/>
-    <mergeCell ref="S39:X40"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="S32:X32"/>
-    <mergeCell ref="B33:O33"/>
-    <mergeCell ref="P33:P34"/>
-    <mergeCell ref="Q33:R34"/>
-    <mergeCell ref="S33:X34"/>
+    <mergeCell ref="V15:W15"/>
     <mergeCell ref="M28:N28"/>
     <mergeCell ref="Q28:S28"/>
     <mergeCell ref="U28:X28"/>
     <mergeCell ref="M29:N29"/>
     <mergeCell ref="Q29:S29"/>
     <mergeCell ref="U29:X29"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="U27:X27"/>
     <mergeCell ref="B10:T10"/>
     <mergeCell ref="W10:X11"/>
     <mergeCell ref="C11:F11"/>
@@ -7792,6 +7792,12 @@
     <mergeCell ref="S13:T13"/>
     <mergeCell ref="V13:W14"/>
     <mergeCell ref="S14:T14"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="U27:X27"/>
     <mergeCell ref="B25:O25"/>
     <mergeCell ref="P25:S25"/>
     <mergeCell ref="T25:X25"/>
@@ -7805,21 +7811,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010049A98165F7642E47B17A8718C6309C3C" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9df6a80b683f270dae4d8a9378e1d1ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0a527c08-909e-4034-a4b4-e3dc69cf1394" xmlns:ns3="ded6c19b-ee5b-4879-90c7-eff5a7dc5c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d0c18106f391fc927c4fcfd7d01849ca" ns2:_="" ns3:_="">
     <xsd:import namespace="0a527c08-909e-4034-a4b4-e3dc69cf1394"/>
@@ -8016,7 +8007,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DE32B7D-BA61-4B9B-A09C-55AF668ACE32}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0a527c08-909e-4034-a4b4-e3dc69cf1394"/>
+    <ds:schemaRef ds:uri="ded6c19b-ee5b-4879-90c7-eff5a7dc5c81"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12F72D6E-F1E6-451F-B825-0462D5FF5E34}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -8033,29 +8058,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98B10ADB-851A-4196-82E8-5B1678715D77}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DE32B7D-BA61-4B9B-A09C-55AF668ACE32}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0a527c08-909e-4034-a4b4-e3dc69cf1394"/>
-    <ds:schemaRef ds:uri="ded6c19b-ee5b-4879-90c7-eff5a7dc5c81"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>